<commit_message>
[add] SoftwareReset and WatchdogTimer
</commit_message>
<xml_diff>
--- a/python/lannerpsp-python test plan 0.0.2.xlsx
+++ b/python/lannerpsp-python test plan 0.0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f15f3a61cb8c2115/Lanner/PSP/psp_api_for_validation/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="13_ncr:1_{8E09B567-5E21-4FC3-ACB1-07791369F630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAFFDCF3-6FB8-4962-B211-BBD71B9D31A6}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="13_ncr:1_{8E09B567-5E21-4FC3-ACB1-07791369F630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C2BAA7C-D5D7-4D5B-970E-FD245F7A331B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="2655" windowWidth="21600" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="2" state="hidden" r:id="rId1"/>
@@ -314,11 +314,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Set LTE Status LED to green blink.
-((./sdk_sled_lte -greenblink)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Set LTE Status LED to yellow.
 (./sdk_sled_lte -yellow)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1178,6 +1173,11 @@
   <si>
     <t>1. Copy paste to IDLE.
 2. Check ??.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set LTE Status LED to green blink.
+(./sdk_sled_lte -greenblink)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1392,6 +1392,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1403,12 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1731,15 +1731,15 @@
       <c r="B4" s="2"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="8" t="s">
@@ -1877,18 +1877,18 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="7" spans="1:10">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="8" t="s">
@@ -1922,7 +1922,7 @@
     </row>
     <row r="9" spans="1:10" ht="94.5">
       <c r="A9" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>44</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="10" spans="1:10" ht="47.25">
       <c r="A10" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>45</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="11" spans="1:10" ht="47.25">
       <c r="A11" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>46</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="12" spans="1:10" ht="47.25">
       <c r="A12" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>47</v>
@@ -2020,18 +2020,18 @@
     </row>
     <row r="14" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="15" spans="1:10">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="8" t="s">
@@ -2065,7 +2065,7 @@
     </row>
     <row r="17" spans="1:10" ht="47.25">
       <c r="A17" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>49</v>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="18" spans="1:10" ht="47.25">
       <c r="A18" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>50</v>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="19" spans="1:10" ht="47.25">
       <c r="A19" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>51</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="20" spans="1:10" ht="47.25">
       <c r="A20" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>52</v>
@@ -2161,18 +2161,18 @@
     </row>
     <row r="22" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="23" spans="1:10">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="8" t="s">
@@ -2206,7 +2206,7 @@
     </row>
     <row r="25" spans="1:10" ht="47.25">
       <c r="A25" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>54</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="26" spans="1:10" ht="47.25">
       <c r="A26" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>55</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="27" spans="1:10" ht="47.25">
       <c r="A27" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>56</v>
@@ -2278,10 +2278,10 @@
     </row>
     <row r="28" spans="1:10" ht="47.25">
       <c r="A28" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>57</v>
+        <v>215</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>15</v>
@@ -2302,10 +2302,10 @@
     </row>
     <row r="29" spans="1:10" ht="47.25">
       <c r="A29" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>15</v>
@@ -2326,10 +2326,10 @@
     </row>
     <row r="30" spans="1:10" ht="47.25">
       <c r="A30" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>15</v>
@@ -2350,10 +2350,10 @@
     </row>
     <row r="31" spans="1:10" ht="47.25">
       <c r="A31" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>15</v>
@@ -2374,10 +2374,10 @@
     </row>
     <row r="32" spans="1:10" ht="47.25">
       <c r="A32" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>15</v>
@@ -2398,18 +2398,18 @@
     </row>
     <row r="34" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="35" spans="1:10">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="8" t="s">
@@ -2443,10 +2443,10 @@
     </row>
     <row r="37" spans="1:10" ht="47.25">
       <c r="A37" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>15</v>
@@ -2455,7 +2455,7 @@
         <v>40</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>21</v>
@@ -2467,10 +2467,10 @@
     </row>
     <row r="38" spans="1:10" ht="47.25">
       <c r="A38" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>15</v>
@@ -2479,7 +2479,7 @@
         <v>41</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>21</v>
@@ -2491,10 +2491,10 @@
     </row>
     <row r="39" spans="1:10" ht="47.25">
       <c r="A39" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>15</v>
@@ -2503,7 +2503,7 @@
         <v>42</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F39" s="11" t="s">
         <v>21</v>
@@ -2515,18 +2515,18 @@
     </row>
     <row r="41" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="42" spans="1:10">
-      <c r="A42" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="22"/>
+      <c r="A42" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="8" t="s">
@@ -2560,22 +2560,22 @@
     </row>
     <row r="44" spans="1:10" ht="47.25">
       <c r="A44" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D44" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="13"/>
@@ -2584,48 +2584,48 @@
     </row>
     <row r="45" spans="1:10" ht="94.5">
       <c r="A45" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G45" s="15"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
       <c r="J45" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="47.25">
       <c r="A46" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="13"/>
@@ -2634,48 +2634,48 @@
     </row>
     <row r="47" spans="1:10" ht="94.5">
       <c r="A47" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="47.25">
       <c r="A48" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="13"/>
@@ -2684,74 +2684,74 @@
     </row>
     <row r="49" spans="1:10" ht="94.5">
       <c r="A49" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="94.5">
       <c r="A50" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="47.25">
       <c r="A51" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="13"/>
@@ -2760,22 +2760,22 @@
     </row>
     <row r="52" spans="1:10" ht="47.25">
       <c r="A52" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="13"/>
@@ -2784,74 +2784,74 @@
     </row>
     <row r="53" spans="1:10" ht="94.5">
       <c r="A53" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="94.5">
       <c r="A54" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
       <c r="J54" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="47.25">
       <c r="A55" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="13"/>
@@ -2860,71 +2860,71 @@
     </row>
     <row r="56" spans="1:10" ht="94.5">
       <c r="A56" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
       <c r="J56" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="94.5">
       <c r="A57" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
       <c r="J57" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="47.25">
       <c r="A58" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B58" s="23" t="s">
-        <v>136</v>
+        <v>183</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>21</v>
@@ -2932,28 +2932,28 @@
       <c r="G58" s="15"/>
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
-      <c r="J58" s="24" t="s">
-        <v>137</v>
+      <c r="J58" s="20" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="47.25">
       <c r="A59" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="13"/>
@@ -2962,18 +2962,18 @@
     </row>
     <row r="61" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="62" spans="1:10">
-      <c r="A62" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="22"/>
+      <c r="A62" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="24"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="8" t="s">
@@ -3007,22 +3007,22 @@
     </row>
     <row r="64" spans="1:10" ht="94.5">
       <c r="A64" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="13"/>
@@ -3031,19 +3031,19 @@
     </row>
     <row r="65" spans="1:10" ht="47.25">
       <c r="A65" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F65" s="11" t="s">
         <v>21</v>
@@ -3055,22 +3055,22 @@
     </row>
     <row r="66" spans="1:10" ht="94.5">
       <c r="A66" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="13"/>
@@ -3079,19 +3079,19 @@
     </row>
     <row r="67" spans="1:10" ht="47.25">
       <c r="A67" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>21</v>
@@ -3103,18 +3103,18 @@
     </row>
     <row r="69" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="70" spans="1:10">
-      <c r="A70" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
-      <c r="J70" s="22"/>
+      <c r="A70" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="24"/>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="8" t="s">
@@ -3148,44 +3148,44 @@
     </row>
     <row r="72" spans="1:10" ht="141.75">
       <c r="A72" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D72" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
       <c r="J72" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="75" spans="1:10">
-      <c r="A75" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B75" s="21"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="21"/>
-      <c r="J75" s="22"/>
+      <c r="A75" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+      <c r="J75" s="24"/>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="8" t="s">
@@ -3219,200 +3219,200 @@
     </row>
     <row r="77" spans="1:10" ht="141.75">
       <c r="A77" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C77" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="141.75">
       <c r="A78" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
       <c r="J78" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="141.75">
       <c r="A79" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C79" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="141.75">
       <c r="A80" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C80" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
       <c r="J80" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="141.75">
       <c r="A81" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C81" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
       <c r="J81" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="141.75">
       <c r="A82" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C82" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
       <c r="J82" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="141.75">
       <c r="A83" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C83" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="13"/>
       <c r="I83" s="13"/>
       <c r="J83" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="16.5" thickBot="1"/>
     <row r="86" spans="1:10">
-      <c r="A86" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
-      <c r="H86" s="21"/>
-      <c r="I86" s="21"/>
-      <c r="J86" s="22"/>
+      <c r="A86" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
+      <c r="J86" s="24"/>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="8" t="s">
@@ -3446,19 +3446,19 @@
     </row>
     <row r="88" spans="1:10" ht="47.25">
       <c r="A88" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C88" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B88" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>199</v>
-      </c>
       <c r="E88" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>21</v>
@@ -3470,19 +3470,19 @@
     </row>
     <row r="89" spans="1:10" ht="47.25">
       <c r="A89" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F89" s="11" t="s">
         <v>21</v>
@@ -3494,19 +3494,19 @@
     </row>
     <row r="90" spans="1:10" ht="47.25">
       <c r="A90" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F90" s="11" t="s">
         <v>21</v>
@@ -3518,19 +3518,19 @@
     </row>
     <row r="91" spans="1:10" ht="47.25">
       <c r="A91" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C91" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F91" s="11" t="s">
         <v>21</v>
@@ -3542,19 +3542,19 @@
     </row>
     <row r="92" spans="1:10" ht="47.25">
       <c r="A92" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C92" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F92" s="11" t="s">
         <v>21</v>

</xml_diff>